<commit_message>
função plano alimentar implementada
</commit_message>
<xml_diff>
--- a/estudo de comportamento de variaves dependentes entre si.xlsx
+++ b/estudo de comportamento de variaves dependentes entre si.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="2370" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
-  <si>
-    <t>peso</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t>kcal</t>
   </si>
@@ -44,9 +41,6 @@
     <t>sedentário</t>
   </si>
   <si>
-    <t>G0</t>
-  </si>
-  <si>
     <t>67.5</t>
   </si>
   <si>
@@ -56,36 +50,6 @@
     <t>40.5</t>
   </si>
   <si>
-    <t>diário</t>
-  </si>
-  <si>
-    <t>3.6</t>
-  </si>
-  <si>
-    <t>2.32</t>
-  </si>
-  <si>
-    <t>23.51</t>
-  </si>
-  <si>
-    <t>2.40</t>
-  </si>
-  <si>
-    <t>5.20</t>
-  </si>
-  <si>
-    <t>0.4</t>
-  </si>
-  <si>
-    <t>0.9</t>
-  </si>
-  <si>
-    <t>2.97</t>
-  </si>
-  <si>
-    <t>0.15</t>
-  </si>
-  <si>
     <t>frango/100g</t>
   </si>
   <si>
@@ -101,10 +65,13 @@
     <t>agua/100ml</t>
   </si>
   <si>
-    <t>Kcal</t>
-  </si>
-  <si>
-    <t>Porção/g</t>
+    <t>macros diários totais</t>
+  </si>
+  <si>
+    <t>whille</t>
+  </si>
+  <si>
+    <t>&lt;</t>
   </si>
 </sst>
 </file>
@@ -140,7 +107,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -148,6 +115,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -428,10 +396,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S6"/>
+  <dimension ref="A1:Q9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+      <selection activeCell="V15" sqref="V15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -441,47 +409,41 @@
     <col min="8" max="8" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="F1" s="3"/>
       <c r="I1" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1" t="s">
         <v>1</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>2</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>3</v>
       </c>
-      <c r="L1" t="s">
-        <v>4</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>25</v>
+      <c r="N1" t="s">
+        <v>0</v>
+      </c>
+      <c r="O1" t="s">
+        <v>1</v>
       </c>
       <c r="P1" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="Q1" t="s">
-        <v>2</v>
-      </c>
-      <c r="R1" t="s">
         <v>3</v>
       </c>
-      <c r="S1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>6</v>
-      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>0</v>
       </c>
@@ -494,11 +456,8 @@
       <c r="E2" t="s">
         <v>3</v>
       </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
       <c r="H2" t="s">
-        <v>20</v>
+        <v>8</v>
       </c>
       <c r="I2" s="1">
         <v>165</v>
@@ -509,101 +468,95 @@
       <c r="K2" s="1">
         <v>0</v>
       </c>
-      <c r="L2" s="1" t="s">
-        <v>11</v>
+      <c r="L2" s="1">
+        <v>3.6</v>
       </c>
       <c r="N2">
-        <v>165</v>
+        <f>SUM(I2:I6)</f>
+        <v>326</v>
+      </c>
+      <c r="O2">
+        <f>SUM(J2:J6)</f>
+        <v>36.619999999999997</v>
       </c>
       <c r="P2">
-        <f>100*N2/$I$2</f>
-        <v>100</v>
+        <f t="shared" ref="O2:Q2" si="0">SUM(K2:K6)</f>
+        <v>31.68</v>
       </c>
       <c r="Q2">
-        <f>100*O2/$I$2</f>
-        <v>0</v>
-      </c>
-      <c r="R2">
-        <f t="shared" ref="Q2:S2" si="0">100*P2/$I$2</f>
-        <v>60.606060606060609</v>
-      </c>
-      <c r="S2">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+        <v>87.15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="1">
+        <v>1175</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="1">
-        <v>50</v>
-      </c>
-      <c r="C3" s="1">
-        <v>1175</v>
-      </c>
       <c r="D3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="H3" t="s">
         <v>9</v>
-      </c>
-      <c r="H3" t="s">
-        <v>21</v>
       </c>
       <c r="I3" s="1">
         <v>112</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K3" s="1" t="s">
-        <v>13</v>
+      <c r="J3" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="K3" s="1">
+        <v>23.51</v>
       </c>
       <c r="L3" s="1">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H4" t="s">
-        <v>22</v>
+        <v>10</v>
       </c>
       <c r="I4" s="1">
         <v>35</v>
       </c>
-      <c r="J4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J4" s="1">
+        <v>2.4</v>
+      </c>
+      <c r="K4" s="1">
+        <v>5.2</v>
+      </c>
+      <c r="L4" s="1">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H5" t="s">
-        <v>23</v>
+        <v>11</v>
       </c>
       <c r="I5" s="1">
         <v>14</v>
       </c>
-      <c r="J5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="L5" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="J5" s="1">
+        <v>0.9</v>
+      </c>
+      <c r="K5" s="1">
+        <v>2.97</v>
+      </c>
+      <c r="L5" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="H6" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="I6" s="1">
         <v>0</v>
@@ -616,11 +569,27 @@
       </c>
       <c r="L6" s="1">
         <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="N9" t="s">
+        <v>14</v>
+      </c>
+      <c r="O9">
+        <f>N2</f>
+        <v>326</v>
+      </c>
+      <c r="P9" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q9">
+        <f>B3</f>
+        <v>1175</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A1:E1"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>

</xml_diff>